<commit_message>
Added crop_images script and updated poly_mask_gen.
</commit_message>
<xml_diff>
--- a/poly_mask_gen.xlsx
+++ b/poly_mask_gen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\calspan1\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02264908-E4CF-43B4-92DB-1F06E0DD5C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3580CB-B41B-4662-AA26-038989A72226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{E2FE00EC-13E0-4EA5-8503-07881E4F671F}"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="28770" windowHeight="15600" xr2:uid="{E2FE00EC-13E0-4EA5-8503-07881E4F671F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1142,7 +1142,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA8FD27D-19C1-35D2-151E-B0BC5B79D99D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1163,6 +1163,67 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4E38FEB-B559-4269-9CB0-594AD536B3A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3095624" y="771524"/>
+          <a:ext cx="5924551" cy="5924551"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1178,7 +1239,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{492E54A5-D4F8-AE0D-7704-BD4F1848A4E6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1187,7 +1248,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:alphaModFix amt="20000"/>
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -1266,7 +1327,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>15</xdr:col>
-          <xdr:colOff>276224</xdr:colOff>
+          <xdr:colOff>276225</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
@@ -1634,7 +1695,7 @@
   <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added violin plot generator.
</commit_message>
<xml_diff>
--- a/poly_mask_gen.xlsx
+++ b/poly_mask_gen.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\calspan1\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3580CB-B41B-4662-AA26-038989A72226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F20C0AB-8E08-4303-B950-C80CD374AB7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="28770" windowHeight="15600" xr2:uid="{E2FE00EC-13E0-4EA5-8503-07881E4F671F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{E2FE00EC-13E0-4EA5-8503-07881E4F671F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$2:$B$36</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$2:$C$36</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -60,12 +65,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -80,8 +91,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,8 +176,10 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -266,6 +280,9 @@
                 <c:pt idx="24">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.10463333333333333</c:v>
+                </c:pt>
                 <c:pt idx="34">
                   <c:v>1</c:v>
                 </c:pt>
@@ -351,6 +368,9 @@
                   <c:v>0.82703333333333329</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="34">
@@ -389,12 +409,7 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -454,12 +469,7 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -509,7 +519,9 @@
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -526,9 +538,7 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="tx1">
@@ -1162,23 +1172,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>346981</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>91167</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>172810</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>110218</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4E38FEB-B559-4269-9CB0-594AD536B3A5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1201,8 +1211,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3095624" y="771524"/>
-          <a:ext cx="5924551" cy="5924551"/>
+          <a:off x="10756445" y="2567667"/>
+          <a:ext cx="5949044" cy="5924551"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1224,15 +1234,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>47627</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>176892</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
+      <xdr:colOff>485777</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>5442</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1251,6 +1261,15 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:alphaModFix amt="20000"/>
           <a:extLst>
+            <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
+              <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a14:imgLayer r:embed="rId4">
+                  <a14:imgEffect>
+                    <a14:sharpenSoften amount="-50000"/>
+                  </a14:imgEffect>
+                </a14:imgLayer>
+              </a14:imgProps>
+            </a:ext>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
@@ -1262,8 +1281,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3095625" y="762000"/>
-          <a:ext cx="5924550" cy="5924550"/>
+          <a:off x="3109234" y="748392"/>
+          <a:ext cx="5949043" cy="5924550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1694,361 +1713,370 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E83D95-7728-4390-87B5-60369455C87F}">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>0.10463333333333333</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>0.17986666666666667</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>0.91203333333333336</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>0.17419999999999999</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>0.83283333333333331</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="1">
         <v>30000</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>0.25813333333333333</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>0.8208333333333333</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>0.34633333333333333</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>0.74226666666666663</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>0.41033333333333333</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>0.7130333333333333</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>0.46396666666666669</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>0.7130333333333333</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>0.50280000000000002</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>0.7200333333333333</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>0.48746666666666666</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>0.70303333333333329</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>0.48246666666666665</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>0.67769999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>0.53293333333333337</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>0.45696666666666669</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>0.49696666666666667</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>0.42049999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>0.49563333333333331</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>0.40483333333333332</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>0.50929999999999997</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>0.39883333333333332</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>0.56856666666666666</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>0.43616666666666665</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>0.57089999999999996</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>0.45483333333333331</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>0.52676666666666672</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>0.67726666666666668</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>0.54443333333333332</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>0.68626666666666669</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>0.57509999999999994</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>0.68459999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>0.59076666666666666</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>0.6992666666666667</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>0.87809999999999999</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>0.79003333333333337</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>0.92443333333333333</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>0.79003333333333337</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>0.96243333333333336</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>0.81336666666666668</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>1</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>0.82703333333333329</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>1</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>25</v>
       </c>
+      <c r="B27" s="1">
+        <v>0.10463333333333333</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="1">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="1">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="1">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="1">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="1">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="1">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="1">
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="1">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="1">
         <v>34</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <f>F40/30000</f>
         <v>1</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <f>Q4/30000</f>
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F40">
+      <c r="F40" s="1">
         <v>30000</v>
       </c>
     </row>

</xml_diff>